<commit_message>
fix buf in show
</commit_message>
<xml_diff>
--- a/test/performance.xlsx
+++ b/test/performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\4-study\FDU\suffermore\DataStructure\HuffmanCompress\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26408EDF-FCDB-4DD0-8880-2FE8A3DBA674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6681E671-7DC4-4BAD-AFFE-E1B8A834A4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14376" yWindow="2711" windowWidth="17425" windowHeight="8555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="351" windowWidth="23452" windowHeight="12827" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>test case</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -175,6 +175,10 @@
   </si>
   <si>
     <t>4.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置：AMD Ryzen 5 4600H 16.0 GB NVIDIA GeForce GTX 1650</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -509,13 +513,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -527,10 +531,10 @@
     <col min="5" max="5" width="16.5546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="30.5546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="24.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="8" max="8" width="55.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -552,8 +556,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -576,7 +583,7 @@
         <v>544.89</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1.2</v>
       </c>
@@ -599,7 +606,7 @@
         <v>12.3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1.3</v>
       </c>
@@ -622,7 +629,7 @@
         <v>16.941299999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1.4</v>
       </c>
@@ -645,7 +652,7 @@
         <v>2.3673999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1.5</v>
       </c>
@@ -668,7 +675,7 @@
         <v>16.009</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.6</v>
       </c>
@@ -691,7 +698,7 @@
         <v>59.357999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1.7</v>
       </c>
@@ -714,7 +721,7 @@
         <v>41.292099999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1.8</v>
       </c>
@@ -737,7 +744,7 @@
         <v>20.072399999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1.9</v>
       </c>
@@ -760,7 +767,7 @@
         <v>468.50799999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -783,7 +790,7 @@
         <v>17.846399999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -806,7 +813,7 @@
         <v>11.663399999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -829,7 +836,7 @@
         <v>17.9651</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -852,7 +859,7 @@
         <v>59.264299999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -875,7 +882,7 @@
         <v>1.6226</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>